<commit_message>
Added additional variables to reflect new education estimates
This commit includes new eductaion estimates and updated columns_number_parameters.xlsx
</commit_message>
<xml_diff>
--- a/input/PL/columns_number_parameters.xlsx
+++ b/input/PL/columns_number_parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pineapple/IdeaProjects/SimPathsEU_NOV/input/PL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pineapple/IdeaProjects/SimPathsEU_testEdu/input/PL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1512C22-DF5B-664E-9051-9BB310F9D1B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17FA3CF-B301-B64C-A649-E4520BA08375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="22760" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36200" yWindow="3560" windowWidth="12980" windowHeight="18100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnsNumberParameters" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>KEY</t>
   </si>
@@ -240,6 +240,15 @@
   </si>
   <si>
     <t>5</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>22</t>
   </si>
 </sst>
 </file>
@@ -613,7 +622,7 @@
   <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -778,24 +787,24 @@
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="1">
-        <v>12</v>
+      <c r="B20" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="1">
-        <v>17</v>
+      <c r="B21" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="1">
-        <v>17</v>
+      <c r="B22" s="4" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated reg_education.xlsx and added additional regressor to Person.java
</commit_message>
<xml_diff>
--- a/input/PL/columns_number_parameters.xlsx
+++ b/input/PL/columns_number_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pineapple/IdeaProjects/SimPathsEU_testEdu/input/PL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17FA3CF-B301-B64C-A649-E4520BA08375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1223FB6-9B7B-4D46-8C5E-629141BC75C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36200" yWindow="3560" windowWidth="12980" windowHeight="18100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32900" yWindow="2940" windowWidth="12980" windowHeight="18100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnsNumberParameters" sheetId="1" r:id="rId1"/>
@@ -242,10 +242,10 @@
     <t>5</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
   </si>
   <si>
     <t>22</t>
@@ -788,7 +788,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -796,7 +796,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated income estimates New income estimates include centered around 20 age variable to avoid a "singular matrix" exception
</commit_message>
<xml_diff>
--- a/input/PL/columns_number_parameters.xlsx
+++ b/input/PL/columns_number_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pineapple/IdeaProjects/SimPathsEU_testEdu/input/PL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DAC4676-2784-EE44-B3C4-1AFF21984892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314507B7-214D-FA43-BA0B-46228FD8573D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32900" yWindow="2940" windowWidth="12980" windowHeight="18100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23900" yWindow="1060" windowWidth="12980" windowHeight="18100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnsNumberParameters" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>KEY</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>20</t>
+  </si>
+  <si>
+    <t>24</t>
   </si>
 </sst>
 </file>
@@ -622,7 +625,7 @@
   <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -859,8 +862,8 @@
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="1">
-        <v>25</v>
+      <c r="B29" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -875,8 +878,8 @@
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="1">
-        <v>25</v>
+      <c r="B31" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated partnership process -Fixed the bug in partnershuo process U2b; -Partnership estimates were updated too.
</commit_message>
<xml_diff>
--- a/input/PL/columns_number_parameters.xlsx
+++ b/input/PL/columns_number_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pineapple/IdeaProjects/SimPathsEU_testEdu/input/PL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314507B7-214D-FA43-BA0B-46228FD8573D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABB9974-4209-2049-9689-F8D08686C2DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23900" yWindow="1060" windowWidth="12980" windowHeight="18100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31580" yWindow="1320" windowWidth="12980" windowHeight="18100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnsNumberParameters" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t>KEY</t>
   </si>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t>24</t>
+  </si>
+  <si>
+    <t>31</t>
   </si>
 </sst>
 </file>
@@ -625,7 +628,7 @@
   <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -822,16 +825,16 @@
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="1">
-        <v>30</v>
+      <c r="B24" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="1">
-        <v>33</v>
+      <c r="B25" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>